<commit_message>
Fixed Art Location for the Switch Button
Part of the VRAM Overhaul
</commit_message>
<xml_diff>
--- a/Assets/PLCs.xlsx
+++ b/Assets/PLCs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="10440"/>
+    <workbookView windowWidth="23040" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="S1 Fixed PLCs" sheetId="9" r:id="rId1"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="153">
   <si>
     <t>Green Hill Zone</t>
   </si>
@@ -559,13 +559,16 @@
     <t>Nem_LZPole</t>
   </si>
   <si>
+    <t>Nem_Flamepipe</t>
+  </si>
+  <si>
     <t>Nem_Squirrel</t>
   </si>
   <si>
     <t>Nem_Jaws</t>
   </si>
   <si>
-    <t>Nem_Flamepipe</t>
+    <t>Nem_SBZWheel1</t>
   </si>
   <si>
     <t>Nem_STH</t>
@@ -574,13 +577,10 @@
     <t>Nem_Burrobot</t>
   </si>
   <si>
-    <t>Nem_SBZWheel1</t>
+    <t>Nem_SBZWheel2</t>
   </si>
   <si>
     <t>SCRATCH (O.W. - Bonus Flags)</t>
-  </si>
-  <si>
-    <t>Nem_SBZWheel2</t>
   </si>
   <si>
     <t>Temporarily placed the SPLASH in this Scratch section</t>
@@ -1890,8 +1890,8 @@
   <sheetPr/>
   <dimension ref="A1:AM60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AF27" sqref="AF27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -4070,7 +4070,7 @@
         <v>30</v>
       </c>
       <c r="AA17" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AB17" s="18" t="str">
         <f ca="1" t="shared" si="15"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="AC17" s="18" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>8760</v>
+        <v>87A0</v>
       </c>
       <c r="AD17" s="18" t="str">
         <f ca="1" t="shared" si="17"/>
@@ -4176,15 +4176,15 @@
       </c>
       <c r="AB18" s="55" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>8760</v>
+        <v>87A0</v>
       </c>
       <c r="AC18" s="55" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>8860</v>
+        <v>88A0</v>
       </c>
       <c r="AD18" s="55" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>43B</v>
+        <v>43D</v>
       </c>
       <c r="AE18" s="57" t="s">
         <v>118</v>
@@ -4251,7 +4251,7 @@
         <v>30</v>
       </c>
       <c r="Q19" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R19" s="18" t="str">
         <f ca="1" t="shared" si="9"/>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="S19" s="18" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>8760</v>
+        <v>87A0</v>
       </c>
       <c r="T19" s="18" t="str">
         <f ca="1" t="shared" si="11"/>
@@ -4270,23 +4270,23 @@
       <c r="W19" s="21"/>
       <c r="X19" s="21"/>
       <c r="Y19" s="21"/>
-      <c r="Z19" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA19" s="18">
-        <v>2</v>
-      </c>
-      <c r="AB19" s="18" t="str">
+      <c r="Z19" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA19" s="55">
+        <v>16</v>
+      </c>
+      <c r="AB19" s="55" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>8860</v>
-      </c>
-      <c r="AC19" s="18" t="str">
+        <v>88A0</v>
+      </c>
+      <c r="AC19" s="55" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>88A0</v>
-      </c>
-      <c r="AD19" s="18" t="str">
+        <v>8AA0</v>
+      </c>
+      <c r="AD19" s="55" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="AE19" s="57" t="s">
         <v>121</v>
@@ -4344,38 +4344,38 @@
       </c>
       <c r="R20" s="47" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>8760</v>
+        <v>87A0</v>
       </c>
       <c r="S20" s="47" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>8860</v>
+        <v>88A0</v>
       </c>
       <c r="T20" s="47" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>43B</v>
+        <v>43D</v>
       </c>
       <c r="U20" s="21"/>
       <c r="V20" s="21"/>
       <c r="W20" s="21"/>
       <c r="X20" s="21"/>
       <c r="Y20" s="21"/>
-      <c r="Z20" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA20" s="55">
-        <v>16</v>
-      </c>
-      <c r="AB20" s="55" t="str">
+      <c r="Z20" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA20" s="59">
+        <v>41</v>
+      </c>
+      <c r="AB20" s="59" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>88A0</v>
-      </c>
-      <c r="AC20" s="55" t="str">
+        <v>8AA0</v>
+      </c>
+      <c r="AC20" s="59" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>8AA0</v>
-      </c>
-      <c r="AD20" s="55" t="str">
+        <v>8FC0</v>
+      </c>
+      <c r="AD20" s="59" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>445</v>
+        <v>455</v>
       </c>
       <c r="AE20" s="57" t="s">
         <v>123</v>
@@ -4420,41 +4420,41 @@
       </c>
       <c r="R21" s="46" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>8860</v>
+        <v>88A0</v>
       </c>
       <c r="S21" s="46" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>8960</v>
+        <v>89A0</v>
       </c>
       <c r="T21" s="46" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
       <c r="X21" s="21"/>
       <c r="Y21" s="21"/>
-      <c r="Z21" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA21" s="59">
-        <v>41</v>
-      </c>
-      <c r="AB21" s="59" t="str">
+      <c r="Z21" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA21" s="53">
+        <v>28</v>
+      </c>
+      <c r="AB21" s="53" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>8AA0</v>
-      </c>
-      <c r="AC21" s="59" t="str">
+        <v>8FC0</v>
+      </c>
+      <c r="AC21" s="53" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>8FC0</v>
-      </c>
-      <c r="AD21" s="59" t="str">
+        <v>9340</v>
+      </c>
+      <c r="AD21" s="53" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>455</v>
+        <v>47E</v>
       </c>
       <c r="AE21" s="57" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AF21" s="57">
         <v>18</v>
@@ -4489,22 +4489,22 @@
       <c r="N22" s="21"/>
       <c r="O22" s="21"/>
       <c r="P22" s="46" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q22" s="46">
         <v>32</v>
       </c>
       <c r="R22" s="46" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>8960</v>
+        <v>89A0</v>
       </c>
       <c r="S22" s="46" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>8D60</v>
+        <v>8DA0</v>
       </c>
       <c r="T22" s="46" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>44B</v>
+        <v>44D</v>
       </c>
       <c r="U22" s="21"/>
       <c r="V22" s="21"/>
@@ -4512,25 +4512,25 @@
       <c r="X22" s="21"/>
       <c r="Y22" s="21"/>
       <c r="Z22" s="53" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AA22" s="53">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="AB22" s="53" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>8FC0</v>
+        <v>9340</v>
       </c>
       <c r="AC22" s="53" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>9340</v>
+        <v>93C0</v>
       </c>
       <c r="AD22" s="53" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>47E</v>
+        <v>49A</v>
       </c>
       <c r="AE22" s="57" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AF22" s="57">
         <v>48</v>
@@ -4565,22 +4565,22 @@
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
       <c r="P23" s="46" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="Q23" s="46">
         <v>90</v>
       </c>
       <c r="R23" s="46" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>8D60</v>
+        <v>8DA0</v>
       </c>
       <c r="S23" s="46" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>98A0</v>
+        <v>98E0</v>
       </c>
       <c r="T23" s="46" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>46B</v>
+        <v>46D</v>
       </c>
       <c r="U23" s="21"/>
       <c r="V23" s="21"/>
@@ -4588,22 +4588,22 @@
       <c r="X23" s="21"/>
       <c r="Y23" s="21"/>
       <c r="Z23" s="53" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AA23" s="53">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="AB23" s="53" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>9340</v>
+        <v>93C0</v>
       </c>
       <c r="AC23" s="53" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>93C0</v>
+        <v>9CE0</v>
       </c>
       <c r="AD23" s="53" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>49A</v>
+        <v>49E</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -4623,14 +4623,14 @@
       <c r="N24" s="21"/>
       <c r="O24" s="21"/>
       <c r="P24" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q24" s="18">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R24" s="18" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>98A0</v>
+        <v>98E0</v>
       </c>
       <c r="S24" s="18" t="str">
         <f ca="1" t="shared" si="10"/>
@@ -4638,33 +4638,33 @@
       </c>
       <c r="T24" s="18" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>4C5</v>
+        <v>4C7</v>
       </c>
       <c r="U24" s="21"/>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
       <c r="X24" s="21"/>
       <c r="Y24" s="21"/>
-      <c r="Z24" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA24" s="53">
-        <v>73</v>
-      </c>
-      <c r="AB24" s="53" t="str">
+      <c r="Z24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA24" s="18">
+        <v>19</v>
+      </c>
+      <c r="AB24" s="18" t="str">
         <f ca="1" t="shared" si="15"/>
-        <v>93C0</v>
-      </c>
-      <c r="AC24" s="53" t="str">
+        <v>9CE0</v>
+      </c>
+      <c r="AC24" s="18" t="str">
         <f ca="1" t="shared" si="16"/>
-        <v>9CE0</v>
-      </c>
-      <c r="AD24" s="53" t="str">
+        <v>9F40</v>
+      </c>
+      <c r="AD24" s="18" t="str">
         <f ca="1" t="shared" si="17"/>
-        <v>49E</v>
+        <v>4E7</v>
       </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -4692,24 +4692,6 @@
       <c r="W25" s="21"/>
       <c r="X25" s="21"/>
       <c r="Y25" s="21"/>
-      <c r="Z25" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA25" s="18">
-        <v>19</v>
-      </c>
-      <c r="AB25" s="18" t="str">
-        <f ca="1" t="shared" si="15"/>
-        <v>9CE0</v>
-      </c>
-      <c r="AC25" s="18" t="str">
-        <f ca="1" t="shared" si="16"/>
-        <v>9F40</v>
-      </c>
-      <c r="AD25" s="18" t="str">
-        <f ca="1" t="shared" si="17"/>
-        <v>4E7</v>
-      </c>
     </row>
     <row r="26" spans="1:25">
       <c r="A26" s="21"/>

</xml_diff>

<commit_message>
Added MZ UFO art from Prototype
Unsure how to implement yet
</commit_message>
<xml_diff>
--- a/Assets/PLCs.xlsx
+++ b/Assets/PLCs.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="154">
   <si>
     <t>Green Hill Zone</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>Nem_Motobug</t>
+  </si>
+  <si>
+    <t>Unc_UFO</t>
   </si>
   <si>
     <t>Nem_Flicky</t>
@@ -1482,8 +1485,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1890,8 +1893,8 @@
   <sheetPr/>
   <dimension ref="A1:AM60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2172,15 +2175,15 @@
         <v>16</v>
       </c>
       <c r="H3" s="8" t="str">
-        <f ca="1" t="shared" ref="H3:H19" si="3">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <f ca="1" t="shared" ref="H3:H20" si="3">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
         <v>52E0</v>
       </c>
       <c r="I3" s="8" t="str">
-        <f ca="1" t="shared" ref="I3:I19" si="4">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
+        <f ca="1" t="shared" ref="I3:I20" si="4">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>54E0</v>
       </c>
       <c r="J3" s="8" t="str">
-        <f ca="1" t="shared" ref="J3:J19" si="5">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <f ca="1" t="shared" ref="J3:J20" si="5">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
         <v>297</v>
       </c>
       <c r="K3" s="41" t="s">
@@ -3928,11 +3931,11 @@
         <f ca="1" t="shared" si="5"/>
         <v>455</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
       <c r="P16" s="46" t="s">
         <v>110</v>
       </c>
@@ -4043,11 +4046,11 @@
         <f ca="1" t="shared" si="5"/>
         <v>492</v>
       </c>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
       <c r="P17" s="47" t="s">
         <v>78</v>
       </c>
@@ -4140,11 +4143,11 @@
         <f ca="1" t="shared" si="5"/>
         <v>4AC</v>
       </c>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
       <c r="P18" s="46" t="s">
         <v>117</v>
       </c>
@@ -4163,11 +4166,11 @@
         <f ca="1" t="shared" si="11"/>
         <v>429</v>
       </c>
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="21"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
       <c r="Z18" s="55" t="s">
         <v>60</v>
       </c>
@@ -4228,7 +4231,7 @@
         <v>120</v>
       </c>
       <c r="G19" s="11">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H19" s="11" t="str">
         <f ca="1" t="shared" si="3"/>
@@ -4236,17 +4239,17 @@
       </c>
       <c r="I19" s="11" t="str">
         <f ca="1" t="shared" si="4"/>
-        <v>9F40</v>
+        <v>9E40</v>
       </c>
       <c r="J19" s="11" t="str">
         <f ca="1" t="shared" si="5"/>
         <v>4C4</v>
       </c>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="20"/>
       <c r="P19" s="18" t="s">
         <v>30</v>
       </c>
@@ -4265,11 +4268,11 @@
         <f ca="1" t="shared" si="11"/>
         <v>439</v>
       </c>
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="W19" s="21"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="20"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="20"/>
       <c r="Z19" s="55" t="s">
         <v>67</v>
       </c>
@@ -4326,16 +4329,29 @@
         <f ca="1" t="shared" si="2"/>
         <v>4DD</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
+      <c r="F20" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="8">
+        <v>8</v>
+      </c>
+      <c r="H20" s="8" t="str">
+        <f ca="1" t="shared" si="3"/>
+        <v>9E40</v>
+      </c>
+      <c r="I20" s="8" t="str">
+        <f ca="1" t="shared" si="4"/>
+        <v>9F40</v>
+      </c>
+      <c r="J20" s="8" t="str">
+        <f ca="1" t="shared" si="5"/>
+        <v>4F2</v>
+      </c>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
       <c r="P20" s="47" t="s">
         <v>60</v>
       </c>
@@ -4354,11 +4370,11 @@
         <f ca="1" t="shared" si="11"/>
         <v>43D</v>
       </c>
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="W20" s="21"/>
-      <c r="X20" s="21"/>
-      <c r="Y20" s="21"/>
+      <c r="U20" s="20"/>
+      <c r="V20" s="20"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="20"/>
+      <c r="Y20" s="20"/>
       <c r="Z20" s="59" t="s">
         <v>73</v>
       </c>
@@ -4378,7 +4394,7 @@
         <v>455</v>
       </c>
       <c r="AE20" s="57" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="AF20" s="57">
         <v>14</v>
@@ -4397,23 +4413,23 @@
       </c>
     </row>
     <row r="21" spans="1:35">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="46" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="Q21" s="46">
         <v>8</v>
@@ -4430,13 +4446,13 @@
         <f ca="1" t="shared" si="11"/>
         <v>445</v>
       </c>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
       <c r="Z21" s="53" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AA21" s="53">
         <v>28</v>
@@ -4454,7 +4470,7 @@
         <v>47E</v>
       </c>
       <c r="AE21" s="57" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AF21" s="57">
         <v>18</v>
@@ -4473,23 +4489,23 @@
       </c>
     </row>
     <row r="22" spans="1:35">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="20"/>
       <c r="P22" s="46" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q22" s="46">
         <v>32</v>
@@ -4506,13 +4522,13 @@
         <f ca="1" t="shared" si="11"/>
         <v>44D</v>
       </c>
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="W22" s="21"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
       <c r="Z22" s="53" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AA22" s="53">
         <v>4</v>
@@ -4530,7 +4546,7 @@
         <v>49A</v>
       </c>
       <c r="AE22" s="57" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AF22" s="57">
         <v>48</v>
@@ -4549,23 +4565,23 @@
       </c>
     </row>
     <row r="23" spans="1:30">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="21"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
       <c r="P23" s="46" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q23" s="46">
         <v>90</v>
@@ -4582,13 +4598,13 @@
         <f ca="1" t="shared" si="11"/>
         <v>46D</v>
       </c>
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="W23" s="21"/>
-      <c r="X23" s="21"/>
-      <c r="Y23" s="21"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
       <c r="Z23" s="53" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AA23" s="53">
         <v>73</v>
@@ -4607,23 +4623,23 @@
       </c>
     </row>
     <row r="24" spans="1:30">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="21"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
       <c r="P24" s="18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Q24" s="18">
         <v>51</v>
@@ -4640,11 +4656,11 @@
         <f ca="1" t="shared" si="11"/>
         <v>4C7</v>
       </c>
-      <c r="U24" s="21"/>
-      <c r="V24" s="21"/>
-      <c r="W24" s="21"/>
-      <c r="X24" s="21"/>
-      <c r="Y24" s="21"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
       <c r="Z24" s="18" t="s">
         <v>30</v>
       </c>
@@ -4665,108 +4681,108 @@
       </c>
     </row>
     <row r="25" spans="1:25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
-      <c r="S25" s="21"/>
-      <c r="T25" s="21"/>
-      <c r="U25" s="21"/>
-      <c r="V25" s="21"/>
-      <c r="W25" s="21"/>
-      <c r="X25" s="21"/>
-      <c r="Y25" s="21"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="21"/>
-      <c r="Q26" s="21"/>
-      <c r="R26" s="21"/>
-      <c r="S26" s="21"/>
-      <c r="T26" s="21"/>
-      <c r="U26" s="21"/>
-      <c r="V26" s="21"/>
-      <c r="W26" s="21"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
     </row>
     <row r="27" s="1" customFormat="1" ht="15.15" spans="1:30">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="22"/>
       <c r="D27" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
       <c r="L27" s="22"/>
       <c r="M27" s="22"/>
       <c r="N27" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O27" s="22"/>
       <c r="P27" s="22"/>
       <c r="Q27" s="22"/>
       <c r="R27" s="22"/>
       <c r="S27" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="T27" s="22"/>
       <c r="U27" s="22"/>
       <c r="V27" s="22"/>
       <c r="W27" s="22"/>
       <c r="X27" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y27" s="22"/>
       <c r="Z27" s="22"/>
       <c r="AA27" s="22"/>
       <c r="AB27" s="22"/>
       <c r="AC27" s="22" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AD27" s="22"/>
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="23" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B28" s="24">
         <v>16</v>
@@ -4784,7 +4800,7 @@
         <v>4FA</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G28" s="24">
         <v>16</v>
@@ -4802,7 +4818,7 @@
         <v>4FA</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L28" s="24">
         <v>16</v>
@@ -4820,7 +4836,7 @@
         <v>4FA</v>
       </c>
       <c r="P28" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q28" s="24">
         <v>16</v>
@@ -4838,7 +4854,7 @@
         <v>4FA</v>
       </c>
       <c r="U28" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="V28" s="24">
         <v>16</v>
@@ -4856,7 +4872,7 @@
         <v>4FA</v>
       </c>
       <c r="Z28" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AA28" s="24">
         <v>16</v>
@@ -4876,7 +4892,7 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B29" s="27">
         <v>14</v>
@@ -4894,7 +4910,7 @@
         <v>50A</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G29" s="27">
         <v>14</v>
@@ -4912,7 +4928,7 @@
         <v>50A</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L29" s="27">
         <v>14</v>
@@ -4930,7 +4946,7 @@
         <v>50A</v>
       </c>
       <c r="P29" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Q29" s="27">
         <v>14</v>
@@ -4948,7 +4964,7 @@
         <v>50A</v>
       </c>
       <c r="U29" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="V29" s="27">
         <v>14</v>
@@ -4966,7 +4982,7 @@
         <v>50A</v>
       </c>
       <c r="Z29" s="27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AA29" s="27">
         <v>14</v>
@@ -4986,7 +5002,7 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B30" s="27">
         <v>10</v>
@@ -5004,7 +5020,7 @@
         <v>518</v>
       </c>
       <c r="F30" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G30" s="27">
         <v>10</v>
@@ -5022,7 +5038,7 @@
         <v>518</v>
       </c>
       <c r="K30" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L30" s="27">
         <v>10</v>
@@ -5040,7 +5056,7 @@
         <v>518</v>
       </c>
       <c r="P30" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Q30" s="27">
         <v>10</v>
@@ -5058,7 +5074,7 @@
         <v>518</v>
       </c>
       <c r="U30" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="V30" s="27">
         <v>10</v>
@@ -5076,7 +5092,7 @@
         <v>518</v>
       </c>
       <c r="Z30" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA30" s="27">
         <v>10</v>
@@ -5096,7 +5112,7 @@
     </row>
     <row r="31" ht="15.15" spans="1:30">
       <c r="A31" s="29" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B31" s="30">
         <v>9</v>
@@ -5114,7 +5130,7 @@
         <v>522</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G31" s="30">
         <v>9</v>
@@ -5132,7 +5148,7 @@
         <v>522</v>
       </c>
       <c r="K31" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L31" s="30">
         <v>9</v>
@@ -5150,7 +5166,7 @@
         <v>522</v>
       </c>
       <c r="P31" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="Q31" s="30">
         <v>9</v>
@@ -5168,7 +5184,7 @@
         <v>522</v>
       </c>
       <c r="U31" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="V31" s="30">
         <v>9</v>
@@ -5186,7 +5202,7 @@
         <v>522</v>
       </c>
       <c r="Z31" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AA31" s="30">
         <v>9</v>
@@ -5206,7 +5222,7 @@
     </row>
     <row r="32" ht="15.6" spans="1:30">
       <c r="A32" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B32" s="32">
         <v>16</v>
@@ -5224,7 +5240,7 @@
         <v>52B</v>
       </c>
       <c r="F32" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G32" s="32">
         <v>16</v>
@@ -5242,7 +5258,7 @@
         <v>52B</v>
       </c>
       <c r="K32" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L32" s="32">
         <v>16</v>
@@ -5260,7 +5276,7 @@
         <v>52B</v>
       </c>
       <c r="P32" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="Q32" s="32">
         <v>16</v>
@@ -5278,7 +5294,7 @@
         <v>52B</v>
       </c>
       <c r="U32" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="V32" s="32">
         <v>16</v>
@@ -5296,7 +5312,7 @@
         <v>52B</v>
       </c>
       <c r="Z32" s="32" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AA32" s="32">
         <v>16</v>
@@ -5315,118 +5331,118 @@
       </c>
     </row>
     <row r="33" spans="1:30">
-      <c r="A33" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="B33" s="21">
+      <c r="A33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="20">
         <v>37</v>
       </c>
-      <c r="C33" s="20" t="str">
+      <c r="C33" s="21" t="str">
         <f ca="1" t="shared" si="21"/>
         <v>A760</v>
       </c>
-      <c r="D33" s="20" t="str">
+      <c r="D33" s="21" t="str">
         <f ca="1" t="shared" si="22"/>
         <v>AC00</v>
       </c>
-      <c r="E33" s="20" t="str">
+      <c r="E33" s="21" t="str">
         <f ca="1" t="shared" si="23"/>
         <v>53B</v>
       </c>
-      <c r="F33" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="G33" s="21">
+      <c r="F33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="20">
         <v>37</v>
       </c>
-      <c r="H33" s="20" t="str">
+      <c r="H33" s="21" t="str">
         <f ca="1" t="shared" si="24"/>
         <v>A760</v>
       </c>
-      <c r="I33" s="20" t="str">
+      <c r="I33" s="21" t="str">
         <f ca="1" t="shared" si="25"/>
         <v>AC00</v>
       </c>
-      <c r="J33" s="20" t="str">
+      <c r="J33" s="21" t="str">
         <f ca="1" t="shared" si="26"/>
         <v>53B</v>
       </c>
-      <c r="K33" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="L33" s="21">
+      <c r="K33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="L33" s="20">
         <v>37</v>
       </c>
-      <c r="M33" s="20" t="str">
+      <c r="M33" s="21" t="str">
         <f ca="1" t="shared" si="27"/>
         <v>A760</v>
       </c>
-      <c r="N33" s="20" t="str">
+      <c r="N33" s="21" t="str">
         <f ca="1" t="shared" si="28"/>
         <v>AC00</v>
       </c>
-      <c r="O33" s="20" t="str">
+      <c r="O33" s="21" t="str">
         <f ca="1" t="shared" si="29"/>
         <v>53B</v>
       </c>
-      <c r="P33" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q33" s="21">
+      <c r="P33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q33" s="20">
         <v>37</v>
       </c>
-      <c r="R33" s="20" t="str">
+      <c r="R33" s="21" t="str">
         <f ca="1" t="shared" si="30"/>
         <v>A760</v>
       </c>
-      <c r="S33" s="20" t="str">
+      <c r="S33" s="21" t="str">
         <f ca="1" t="shared" si="31"/>
         <v>AC00</v>
       </c>
-      <c r="T33" s="20" t="str">
+      <c r="T33" s="21" t="str">
         <f ca="1" t="shared" si="32"/>
         <v>53B</v>
       </c>
-      <c r="U33" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="V33" s="21">
+      <c r="U33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="V33" s="20">
         <v>37</v>
       </c>
-      <c r="W33" s="20" t="str">
+      <c r="W33" s="21" t="str">
         <f ca="1" t="shared" si="33"/>
         <v>A760</v>
       </c>
-      <c r="X33" s="20" t="str">
+      <c r="X33" s="21" t="str">
         <f ca="1" t="shared" si="34"/>
         <v>AC00</v>
       </c>
-      <c r="Y33" s="20" t="str">
+      <c r="Y33" s="21" t="str">
         <f ca="1" t="shared" si="35"/>
         <v>53B</v>
       </c>
-      <c r="Z33" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA33" s="21">
+      <c r="Z33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA33" s="20">
         <v>37</v>
       </c>
-      <c r="AB33" s="20" t="str">
+      <c r="AB33" s="21" t="str">
         <f ca="1" t="shared" si="36"/>
         <v>A760</v>
       </c>
-      <c r="AC33" s="20" t="str">
+      <c r="AC33" s="21" t="str">
         <f ca="1" t="shared" si="37"/>
         <v>AC00</v>
       </c>
-      <c r="AD33" s="20" t="str">
+      <c r="AD33" s="21" t="str">
         <f ca="1" t="shared" si="38"/>
         <v>53B</v>
       </c>
     </row>
     <row r="34" ht="15.15" spans="1:30">
       <c r="A34" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B34" s="1">
         <v>8</v>
@@ -5444,7 +5460,7 @@
         <v>560</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G34" s="1">
         <v>8</v>
@@ -5462,7 +5478,7 @@
         <v>560</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="L34" s="1">
         <v>8</v>
@@ -5480,7 +5496,7 @@
         <v>560</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q34" s="1">
         <v>8</v>
@@ -5498,7 +5514,7 @@
         <v>560</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="V34" s="1">
         <v>8</v>
@@ -5516,7 +5532,7 @@
         <v>560</v>
       </c>
       <c r="Z34" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AA34" s="1">
         <v>8</v>
@@ -5536,7 +5552,7 @@
     </row>
     <row r="35" spans="1:30">
       <c r="A35" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B35" s="25">
         <v>36</v>
@@ -5554,7 +5570,7 @@
         <v>568</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G35" s="25">
         <v>36</v>
@@ -5572,7 +5588,7 @@
         <v>568</v>
       </c>
       <c r="K35" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L35" s="25">
         <v>36</v>
@@ -5590,7 +5606,7 @@
         <v>568</v>
       </c>
       <c r="P35" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q35" s="25">
         <v>36</v>
@@ -5608,7 +5624,7 @@
         <v>568</v>
       </c>
       <c r="U35" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="V35" s="25">
         <v>36</v>
@@ -5626,7 +5642,7 @@
         <v>568</v>
       </c>
       <c r="Z35" s="33" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AA35" s="25">
         <v>36</v>
@@ -5646,7 +5662,7 @@
     </row>
     <row r="36" spans="1:30">
       <c r="A36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B36" s="28">
         <v>96</v>
@@ -5664,7 +5680,7 @@
         <v>58C</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G36" s="28">
         <v>96</v>
@@ -5682,7 +5698,7 @@
         <v>58C</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="L36" s="28">
         <v>96</v>
@@ -5700,7 +5716,7 @@
         <v>58C</v>
       </c>
       <c r="P36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Q36" s="28">
         <v>96</v>
@@ -5718,7 +5734,7 @@
         <v>58C</v>
       </c>
       <c r="U36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="V36" s="28">
         <v>96</v>
@@ -5736,7 +5752,7 @@
         <v>58C</v>
       </c>
       <c r="Z36" s="34" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AA36" s="28">
         <v>96</v>
@@ -5756,7 +5772,7 @@
     </row>
     <row r="37" spans="1:30">
       <c r="A37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1">
         <v>20</v>
@@ -5774,7 +5790,7 @@
         <v>5EC</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G37" s="1">
         <v>20</v>
@@ -5792,7 +5808,7 @@
         <v>5EC</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L37" s="1">
         <v>20</v>
@@ -5810,7 +5826,7 @@
         <v>5EC</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Q37" s="1">
         <v>20</v>
@@ -5828,7 +5844,7 @@
         <v>5EC</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="V37" s="1">
         <v>20</v>
@@ -5846,7 +5862,7 @@
         <v>5EC</v>
       </c>
       <c r="Z37" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA37" s="1">
         <v>20</v>
@@ -5866,7 +5882,7 @@
     </row>
     <row r="38" spans="1:30">
       <c r="A38" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B38" s="35">
         <v>128</v>
@@ -5884,7 +5900,7 @@
         <v>600</v>
       </c>
       <c r="F38" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G38" s="35">
         <v>128</v>
@@ -5902,7 +5918,7 @@
         <v>600</v>
       </c>
       <c r="K38" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L38" s="35">
         <v>128</v>
@@ -5920,7 +5936,7 @@
         <v>600</v>
       </c>
       <c r="P38" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="Q38" s="35">
         <v>128</v>
@@ -5938,7 +5954,7 @@
         <v>600</v>
       </c>
       <c r="U38" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="V38" s="35">
         <v>128</v>
@@ -5956,7 +5972,7 @@
         <v>600</v>
       </c>
       <c r="Z38" s="35" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AA38" s="35">
         <v>128</v>
@@ -5976,7 +5992,7 @@
     </row>
     <row r="39" spans="1:30">
       <c r="A39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B39" s="1">
         <v>74</v>
@@ -5994,7 +6010,7 @@
         <v>680</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G39" s="1">
         <v>74</v>
@@ -6012,7 +6028,7 @@
         <v>680</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="L39" s="1">
         <v>74</v>
@@ -6030,7 +6046,7 @@
         <v>680</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q39" s="1">
         <v>74</v>
@@ -6048,7 +6064,7 @@
         <v>680</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="V39" s="1">
         <v>74</v>
@@ -6066,7 +6082,7 @@
         <v>680</v>
       </c>
       <c r="Z39" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AA39" s="1">
         <v>74</v>
@@ -6086,7 +6102,7 @@
     </row>
     <row r="40" spans="1:30">
       <c r="A40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B40" s="36">
         <v>54</v>
@@ -6104,7 +6120,7 @@
         <v>6CA</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G40" s="36">
         <v>54</v>
@@ -6122,7 +6138,7 @@
         <v>6CA</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L40" s="36">
         <v>54</v>
@@ -6140,7 +6156,7 @@
         <v>6CA</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="Q40" s="36">
         <v>54</v>
@@ -6158,7 +6174,7 @@
         <v>6CA</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="V40" s="36">
         <v>54</v>
@@ -6176,7 +6192,7 @@
         <v>6CA</v>
       </c>
       <c r="Z40" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AA40" s="36">
         <v>54</v>
@@ -6196,7 +6212,7 @@
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B41" s="35">
         <v>128</v>
@@ -6214,7 +6230,7 @@
         <v>700</v>
       </c>
       <c r="F41" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G41" s="35">
         <v>128</v>
@@ -6232,7 +6248,7 @@
         <v>700</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="L41" s="35">
         <v>128</v>
@@ -6250,7 +6266,7 @@
         <v>700</v>
       </c>
       <c r="P41" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Q41" s="35">
         <v>128</v>
@@ -6268,7 +6284,7 @@
         <v>700</v>
       </c>
       <c r="U41" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="V41" s="35">
         <v>128</v>
@@ -6286,7 +6302,7 @@
         <v>700</v>
       </c>
       <c r="Z41" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AA41" s="35">
         <v>128</v>
@@ -6306,7 +6322,7 @@
     </row>
     <row r="42" spans="1:30">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B42">
         <v>32</v>
@@ -6324,7 +6340,7 @@
         <v>780</v>
       </c>
       <c r="F42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G42">
         <v>32</v>
@@ -6342,7 +6358,7 @@
         <v>780</v>
       </c>
       <c r="K42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L42">
         <v>32</v>
@@ -6360,7 +6376,7 @@
         <v>780</v>
       </c>
       <c r="P42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q42">
         <v>32</v>
@@ -6378,7 +6394,7 @@
         <v>780</v>
       </c>
       <c r="U42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="V42">
         <v>32</v>
@@ -6396,7 +6412,7 @@
         <v>780</v>
       </c>
       <c r="Z42" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AA42">
         <v>32</v>
@@ -6526,7 +6542,7 @@
     </row>
     <row r="44" spans="1:30">
       <c r="A44" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B44" s="35">
         <v>20</v>
@@ -6544,7 +6560,7 @@
         <v>7C0</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G44" s="35">
         <v>20</v>
@@ -6562,7 +6578,7 @@
         <v>7C0</v>
       </c>
       <c r="K44" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="L44" s="35">
         <v>20</v>
@@ -6580,7 +6596,7 @@
         <v>7C0</v>
       </c>
       <c r="P44" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="Q44" s="35">
         <v>20</v>
@@ -6598,7 +6614,7 @@
         <v>7C0</v>
       </c>
       <c r="U44" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="V44" s="35">
         <v>20</v>
@@ -6616,7 +6632,7 @@
         <v>7C0</v>
       </c>
       <c r="Z44" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AA44" s="35">
         <v>20</v>
@@ -6635,118 +6651,118 @@
       </c>
     </row>
     <row r="45" spans="1:30">
-      <c r="A45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="B45" s="21">
+      <c r="A45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="20">
         <v>12</v>
       </c>
-      <c r="C45" s="20" t="str">
+      <c r="C45" s="21" t="str">
         <f ca="1" t="shared" si="39"/>
         <v>FA80</v>
       </c>
-      <c r="D45" s="20" t="str">
+      <c r="D45" s="21" t="str">
         <f ca="1" t="shared" si="40"/>
         <v>FC00</v>
       </c>
-      <c r="E45" s="20" t="str">
+      <c r="E45" s="21" t="str">
         <f ca="1" t="shared" si="41"/>
         <v>7D4</v>
       </c>
-      <c r="F45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="G45" s="21">
+      <c r="F45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G45" s="20">
         <v>12</v>
       </c>
-      <c r="H45" s="20" t="str">
+      <c r="H45" s="21" t="str">
         <f ca="1" t="shared" si="42"/>
         <v>FA80</v>
       </c>
-      <c r="I45" s="20" t="str">
+      <c r="I45" s="21" t="str">
         <f ca="1" t="shared" si="43"/>
         <v>FC00</v>
       </c>
-      <c r="J45" s="20" t="str">
+      <c r="J45" s="21" t="str">
         <f ca="1" t="shared" si="44"/>
         <v>7D4</v>
       </c>
-      <c r="K45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="L45" s="21">
+      <c r="K45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="L45" s="20">
         <v>12</v>
       </c>
-      <c r="M45" s="20" t="str">
+      <c r="M45" s="21" t="str">
         <f ca="1" t="shared" si="45"/>
         <v>FA80</v>
       </c>
-      <c r="N45" s="20" t="str">
+      <c r="N45" s="21" t="str">
         <f ca="1" t="shared" si="46"/>
         <v>FC00</v>
       </c>
-      <c r="O45" s="20" t="str">
+      <c r="O45" s="21" t="str">
         <f ca="1" t="shared" si="47"/>
         <v>7D4</v>
       </c>
-      <c r="P45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q45" s="21">
+      <c r="P45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q45" s="20">
         <v>12</v>
       </c>
-      <c r="R45" s="20" t="str">
+      <c r="R45" s="21" t="str">
         <f ca="1" t="shared" si="48"/>
         <v>FA80</v>
       </c>
-      <c r="S45" s="20" t="str">
+      <c r="S45" s="21" t="str">
         <f ca="1" t="shared" si="49"/>
         <v>FC00</v>
       </c>
-      <c r="T45" s="20" t="str">
+      <c r="T45" s="21" t="str">
         <f ca="1" t="shared" si="50"/>
         <v>7D4</v>
       </c>
-      <c r="U45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="V45" s="21">
+      <c r="U45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="V45" s="20">
         <v>12</v>
       </c>
-      <c r="W45" s="20" t="str">
+      <c r="W45" s="21" t="str">
         <f ca="1" t="shared" si="51"/>
         <v>FA80</v>
       </c>
-      <c r="X45" s="20" t="str">
+      <c r="X45" s="21" t="str">
         <f ca="1" t="shared" si="52"/>
         <v>FC00</v>
       </c>
-      <c r="Y45" s="20" t="str">
+      <c r="Y45" s="21" t="str">
         <f ca="1" t="shared" si="53"/>
         <v>7D4</v>
       </c>
-      <c r="Z45" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA45" s="21">
+      <c r="Z45" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA45" s="20">
         <v>12</v>
       </c>
-      <c r="AB45" s="20" t="str">
+      <c r="AB45" s="21" t="str">
         <f ca="1" t="shared" si="54"/>
         <v>FA80</v>
       </c>
-      <c r="AC45" s="20" t="str">
+      <c r="AC45" s="21" t="str">
         <f ca="1" t="shared" si="55"/>
         <v>FC00</v>
       </c>
-      <c r="AD45" s="20" t="str">
+      <c r="AD45" s="21" t="str">
         <f ca="1" t="shared" si="56"/>
         <v>7D4</v>
       </c>
     </row>
     <row r="46" spans="1:30">
       <c r="A46" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B46" s="35">
         <v>32</v>
@@ -6764,7 +6780,7 @@
         <v>7E0</v>
       </c>
       <c r="F46" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G46" s="35">
         <v>32</v>
@@ -6782,7 +6798,7 @@
         <v>7E0</v>
       </c>
       <c r="K46" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="L46" s="35">
         <v>32</v>
@@ -6800,7 +6816,7 @@
         <v>7E0</v>
       </c>
       <c r="P46" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q46" s="35">
         <v>32</v>
@@ -6818,7 +6834,7 @@
         <v>7E0</v>
       </c>
       <c r="U46" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="V46" s="35">
         <v>32</v>
@@ -6836,7 +6852,7 @@
         <v>7E0</v>
       </c>
       <c r="Z46" s="35" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AA46" s="35">
         <v>32</v>

</xml_diff>

<commit_message>
New SBZ3 Burrobot Art (RetroKoH)
Removed one unused Burrobot Frame and associated art tiles ($5A tiles -> $4B tiles)
</commit_message>
<xml_diff>
--- a/Assets/PLCs.xlsx
+++ b/Assets/PLCs.xlsx
@@ -1893,8 +1893,8 @@
   <sheetPr/>
   <dimension ref="A1:AM60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -4584,7 +4584,7 @@
         <v>131</v>
       </c>
       <c r="Q23" s="46">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="R23" s="46" t="str">
         <f ca="1" t="shared" si="9"/>
@@ -4592,7 +4592,7 @@
       </c>
       <c r="S23" s="46" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>98E0</v>
+        <v>9700</v>
       </c>
       <c r="T23" s="46" t="str">
         <f ca="1" t="shared" si="11"/>
@@ -4642,11 +4642,11 @@
         <v>133</v>
       </c>
       <c r="Q24" s="18">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="R24" s="18" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>98E0</v>
+        <v>9700</v>
       </c>
       <c r="S24" s="18" t="str">
         <f ca="1" t="shared" si="10"/>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="T24" s="18" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>4C7</v>
+        <v>4B8</v>
       </c>
       <c r="U24" s="20"/>
       <c r="V24" s="20"/>

</xml_diff>

<commit_message>
LZ Conveyor Wheel Optimized (RetroKoH)
</commit_message>
<xml_diff>
--- a/Assets/PLCs.xlsx
+++ b/Assets/PLCs.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="154">
   <si>
     <t>Green Hill Zone</t>
   </si>
@@ -499,7 +499,7 @@
     <t>Nem_EndSonic</t>
   </si>
   <si>
-    <t>Nem_LZWheel</t>
+    <t>Nem_LZConveyorWheel/Ptfm</t>
   </si>
   <si>
     <t>Nem_SLZBlock</t>
@@ -514,18 +514,18 @@
     <t>Nem_Chopper</t>
   </si>
   <si>
+    <t>Nem_SpinPlatform</t>
+  </si>
+  <si>
+    <t>Nem_Chicken</t>
+  </si>
+  <si>
+    <t>Nem_MZGlass</t>
+  </si>
+  <si>
     <t>Nem_LZPlatfm</t>
   </si>
   <si>
-    <t>Nem_SpinPlatform</t>
-  </si>
-  <si>
-    <t>Nem_Chicken</t>
-  </si>
-  <si>
-    <t>Nem_MZGlass</t>
-  </si>
-  <si>
     <t>Nem_Penguin</t>
   </si>
   <si>
@@ -535,18 +535,18 @@
     <t>Nem_MZBlock</t>
   </si>
   <si>
+    <t>Nem_Seal</t>
+  </si>
+  <si>
+    <t>Nem_Newtron</t>
+  </si>
+  <si>
+    <t>SCRATCH  (O.W. - Bonus Flags)</t>
+  </si>
+  <si>
     <t>Nem_Cork</t>
   </si>
   <si>
-    <t>Nem_Seal</t>
-  </si>
-  <si>
-    <t>Nem_Newtron</t>
-  </si>
-  <si>
-    <t>SCRATCH  (O.W. - Bonus Flags)</t>
-  </si>
-  <si>
     <t>Nem_Pig</t>
   </si>
   <si>
@@ -559,28 +559,28 @@
     <t>Nem_Flicky</t>
   </si>
   <si>
+    <t>Nem_Flamepipe</t>
+  </si>
+  <si>
+    <t>Nem_Squirrel</t>
+  </si>
+  <si>
     <t>Nem_LZPole</t>
   </si>
   <si>
-    <t>Nem_Flamepipe</t>
-  </si>
-  <si>
-    <t>Nem_Squirrel</t>
+    <t>Nem_SBZWheel1</t>
+  </si>
+  <si>
+    <t>Nem_STH</t>
   </si>
   <si>
     <t>Nem_Jaws</t>
   </si>
   <si>
-    <t>Nem_SBZWheel1</t>
-  </si>
-  <si>
-    <t>Nem_STH</t>
+    <t>Nem_SBZWheel2</t>
   </si>
   <si>
     <t>Nem_Burrobot</t>
-  </si>
-  <si>
-    <t>Nem_SBZWheel2</t>
   </si>
   <si>
     <t>SCRATCH (O.W. - Bonus Flags)</t>
@@ -1893,8 +1893,8 @@
   <sheetPr/>
   <dimension ref="A1:AM60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -3825,7 +3825,7 @@
         <v>105</v>
       </c>
       <c r="Q15" s="46">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="R15" s="46" t="str">
         <f ca="1" t="shared" si="9"/>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="S15" s="46" t="str">
         <f ca="1" t="shared" si="10"/>
-        <v>7E40</v>
+        <v>7840</v>
       </c>
       <c r="T15" s="46" t="str">
         <f ca="1" t="shared" si="11"/>
@@ -3936,23 +3936,23 @@
       <c r="M16" s="20"/>
       <c r="N16" s="20"/>
       <c r="O16" s="20"/>
-      <c r="P16" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q16" s="46">
-        <v>24</v>
-      </c>
-      <c r="R16" s="46" t="str">
+      <c r="P16" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" s="18">
+        <v>48</v>
+      </c>
+      <c r="R16" s="18" t="str">
         <f ca="1" t="shared" si="9"/>
+        <v>7840</v>
+      </c>
+      <c r="S16" s="18" t="str">
+        <f ca="1" t="shared" si="10"/>
         <v>7E40</v>
       </c>
-      <c r="S16" s="46" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>8140</v>
-      </c>
-      <c r="T16" s="46" t="str">
+      <c r="T16" s="18" t="str">
         <f ca="1" t="shared" si="11"/>
-        <v>3F2</v>
+        <v>3C2</v>
       </c>
       <c r="U16" s="18" t="s">
         <v>30</v>
@@ -3973,7 +3973,7 @@
         <v>49E</v>
       </c>
       <c r="Z16" s="58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AA16" s="58">
         <v>48</v>
@@ -3991,7 +3991,7 @@
         <v>401</v>
       </c>
       <c r="AE16" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AF16" s="57">
         <v>14</v>
@@ -4029,7 +4029,7 @@
         <v>45D</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G17" s="8">
         <v>26</v>
@@ -4051,23 +4051,23 @@
       <c r="M17" s="20"/>
       <c r="N17" s="20"/>
       <c r="O17" s="20"/>
-      <c r="P17" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q17" s="47">
-        <v>31</v>
-      </c>
-      <c r="R17" s="47" t="str">
-        <f ca="1" t="shared" si="9"/>
+      <c r="P17" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q17" s="46">
+        <v>24</v>
+      </c>
+      <c r="R17" s="46" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>7E40</v>
+      </c>
+      <c r="S17" s="46" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>8140</v>
       </c>
-      <c r="S17" s="47" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>8520</v>
-      </c>
-      <c r="T17" s="47" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>40A</v>
+      <c r="T17" s="46" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>3F2</v>
       </c>
       <c r="Z17" s="18" t="s">
         <v>30</v>
@@ -4148,23 +4148,23 @@
       <c r="M18" s="20"/>
       <c r="N18" s="20"/>
       <c r="O18" s="20"/>
-      <c r="P18" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q18" s="46">
-        <v>16</v>
-      </c>
-      <c r="R18" s="46" t="str">
-        <f ca="1" t="shared" si="9"/>
+      <c r="P18" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q18" s="47">
+        <v>31</v>
+      </c>
+      <c r="R18" s="47" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>8140</v>
+      </c>
+      <c r="S18" s="47" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>8520</v>
       </c>
-      <c r="S18" s="46" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>8720</v>
-      </c>
-      <c r="T18" s="46" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>429</v>
+      <c r="T18" s="47" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>40A</v>
       </c>
       <c r="U18" s="20"/>
       <c r="V18" s="20"/>
@@ -4190,7 +4190,7 @@
         <v>43D</v>
       </c>
       <c r="AE18" s="57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AF18" s="57">
         <v>14</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="19" spans="1:35">
       <c r="A19" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19" s="13">
         <v>85</v>
@@ -4228,7 +4228,7 @@
         <v>488</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="11">
         <v>46</v>
@@ -4250,23 +4250,23 @@
       <c r="M19" s="20"/>
       <c r="N19" s="20"/>
       <c r="O19" s="20"/>
-      <c r="P19" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q19" s="18">
-        <v>4</v>
-      </c>
-      <c r="R19" s="18" t="str">
-        <f ca="1" t="shared" si="9"/>
+      <c r="P19" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q19" s="46">
+        <v>16</v>
+      </c>
+      <c r="R19" s="46" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>8520</v>
+      </c>
+      <c r="S19" s="46" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>8720</v>
       </c>
-      <c r="S19" s="18" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>87A0</v>
-      </c>
-      <c r="T19" s="18" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>439</v>
+      <c r="T19" s="46" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>429</v>
       </c>
       <c r="U19" s="20"/>
       <c r="V19" s="20"/>
@@ -4352,23 +4352,23 @@
       <c r="M20" s="20"/>
       <c r="N20" s="20"/>
       <c r="O20" s="20"/>
-      <c r="P20" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q20" s="44">
-        <v>8</v>
-      </c>
-      <c r="R20" s="47" t="str">
-        <f ca="1" t="shared" si="9"/>
+      <c r="P20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="18">
+        <v>4</v>
+      </c>
+      <c r="R20" s="18" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>8720</v>
+      </c>
+      <c r="S20" s="18" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>87A0</v>
       </c>
-      <c r="S20" s="47" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>88A0</v>
-      </c>
-      <c r="T20" s="47" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>43D</v>
+      <c r="T20" s="18" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>439</v>
       </c>
       <c r="U20" s="20"/>
       <c r="V20" s="20"/>
@@ -4428,23 +4428,23 @@
       <c r="M21" s="20"/>
       <c r="N21" s="20"/>
       <c r="O21" s="20"/>
-      <c r="P21" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q21" s="46">
+      <c r="P21" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q21" s="44">
         <v>8</v>
       </c>
-      <c r="R21" s="46" t="str">
-        <f ca="1" t="shared" si="9"/>
+      <c r="R21" s="47" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>87A0</v>
+      </c>
+      <c r="S21" s="47" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>88A0</v>
       </c>
-      <c r="S21" s="46" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>89A0</v>
-      </c>
-      <c r="T21" s="46" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>445</v>
+      <c r="T21" s="47" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>43D</v>
       </c>
       <c r="U21" s="20"/>
       <c r="V21" s="20"/>
@@ -4452,7 +4452,7 @@
       <c r="X21" s="20"/>
       <c r="Y21" s="20"/>
       <c r="Z21" s="53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AA21" s="53">
         <v>28</v>
@@ -4470,7 +4470,7 @@
         <v>47E</v>
       </c>
       <c r="AE21" s="57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AF21" s="57">
         <v>18</v>
@@ -4505,22 +4505,22 @@
       <c r="N22" s="20"/>
       <c r="O22" s="20"/>
       <c r="P22" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Q22" s="46">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="R22" s="46" t="str">
-        <f ca="1" t="shared" si="9"/>
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>88A0</v>
+      </c>
+      <c r="S22" s="46" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>89A0</v>
       </c>
-      <c r="S22" s="46" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>8DA0</v>
-      </c>
       <c r="T22" s="46" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>44D</v>
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>445</v>
       </c>
       <c r="U22" s="20"/>
       <c r="V22" s="20"/>
@@ -4528,7 +4528,7 @@
       <c r="X22" s="20"/>
       <c r="Y22" s="20"/>
       <c r="Z22" s="53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AA22" s="53">
         <v>4</v>
@@ -4546,7 +4546,7 @@
         <v>49A</v>
       </c>
       <c r="AE22" s="57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AF22" s="57">
         <v>48</v>
@@ -4581,22 +4581,22 @@
       <c r="N23" s="20"/>
       <c r="O23" s="20"/>
       <c r="P23" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q23" s="46">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="R23" s="46" t="str">
-        <f ca="1" t="shared" si="9"/>
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>89A0</v>
+      </c>
+      <c r="S23" s="46" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>8DA0</v>
       </c>
-      <c r="S23" s="46" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>9700</v>
-      </c>
       <c r="T23" s="46" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>46D</v>
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>44D</v>
       </c>
       <c r="U23" s="20"/>
       <c r="V23" s="20"/>
@@ -4604,7 +4604,7 @@
       <c r="X23" s="20"/>
       <c r="Y23" s="20"/>
       <c r="Z23" s="53" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AA23" s="53">
         <v>73</v>
@@ -4638,23 +4638,23 @@
       <c r="M24" s="20"/>
       <c r="N24" s="20"/>
       <c r="O24" s="20"/>
-      <c r="P24" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q24" s="18">
-        <v>66</v>
-      </c>
-      <c r="R24" s="18" t="str">
-        <f ca="1" t="shared" si="9"/>
+      <c r="P24" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q24" s="46">
+        <v>75</v>
+      </c>
+      <c r="R24" s="46" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>8DA0</v>
+      </c>
+      <c r="S24" s="46" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
         <v>9700</v>
       </c>
-      <c r="S24" s="18" t="str">
-        <f ca="1" t="shared" si="10"/>
-        <v>9F40</v>
-      </c>
-      <c r="T24" s="18" t="str">
-        <f ca="1" t="shared" si="11"/>
-        <v>4B8</v>
+      <c r="T24" s="46" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>46D</v>
       </c>
       <c r="U24" s="20"/>
       <c r="V24" s="20"/>
@@ -4696,13 +4696,24 @@
       <c r="M25" s="20"/>
       <c r="N25" s="20"/>
       <c r="O25" s="20"/>
-      <c r="P25" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="20"/>
+      <c r="P25" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>66</v>
+      </c>
+      <c r="R25" s="18" t="str">
+        <f ca="1">OFFSET(INDIRECT("RC",FALSE),-1,1)</f>
+        <v>9700</v>
+      </c>
+      <c r="S25" s="18" t="str">
+        <f ca="1">DEC2HEX(PRODUCT(OFFSET(INDIRECT("RC",FALSE),0,-2),32)+HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-1)),4)</f>
+        <v>9F40</v>
+      </c>
+      <c r="T25" s="18" t="str">
+        <f ca="1">DEC2HEX(HEX2DEC(OFFSET(INDIRECT("RC",FALSE),0,-2))/32)</f>
+        <v>4B8</v>
+      </c>
       <c r="U25" s="20"/>
       <c r="V25" s="20"/>
       <c r="W25" s="20"/>
@@ -4725,7 +4736,9 @@
       <c r="M26" s="20"/>
       <c r="N26" s="20"/>
       <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
+      <c r="P26" s="20" t="s">
+        <v>134</v>
+      </c>
       <c r="Q26" s="20"/>
       <c r="R26" s="20"/>
       <c r="S26" s="20"/>

</xml_diff>